<commit_message>
Proyecto final casi completo, solo falta poner bien las rutas
</commit_message>
<xml_diff>
--- a/planos/all_images/split/test/images/results_sensores/10_flip_sensors.xlsx
+++ b/planos/all_images/split/test/images/results_sensores/10_flip_sensors.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>19.13697403890975</v>
+        <v>19.12497595493468</v>
       </c>
       <c r="F2" t="n">
-        <v>1.831856813222433</v>
+        <v>1.830708315459377</v>
       </c>
       <c r="G2" t="n">
         <v>0.1</v>
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8.063607474994274</v>
+        <v>8.0585519296698</v>
       </c>
       <c r="F3" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G3" t="n">
         <v>0.1</v>
@@ -554,10 +554,10 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>8.063607474994274</v>
+        <v>8.0585519296698</v>
       </c>
       <c r="F4" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G4" t="n">
         <v>0.6</v>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8.063607474994274</v>
+        <v>8.0585519296698</v>
       </c>
       <c r="F5" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -616,10 +616,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8.063607474994274</v>
+        <v>8.0585519296698</v>
       </c>
       <c r="F6" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G6" t="n">
         <v>1.1</v>
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>10.35055948581328</v>
+        <v>10.34407011703182</v>
       </c>
       <c r="F7" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G7" t="n">
         <v>0.1</v>
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>10.35055948581328</v>
+        <v>10.34407011703182</v>
       </c>
       <c r="F8" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G8" t="n">
         <v>0.6</v>
@@ -709,10 +709,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>10.35055948581328</v>
+        <v>10.34407011703182</v>
       </c>
       <c r="F9" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -740,10 +740,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>10.35055948581328</v>
+        <v>10.34407011703182</v>
       </c>
       <c r="F10" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G10" t="n">
         <v>1.1</v>
@@ -771,10 +771,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>9.207083480403778</v>
+        <v>9.201311023350812</v>
       </c>
       <c r="F11" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G11" t="n">
         <v>0.1</v>
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>9.207083480403778</v>
+        <v>9.201311023350812</v>
       </c>
       <c r="F12" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G12" t="n">
         <v>1.1</v>
@@ -833,10 +833,10 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>9.207083480403778</v>
+        <v>9.201311023350812</v>
       </c>
       <c r="F13" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G13" t="n">
         <v>1.7</v>
@@ -864,10 +864,10 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>9.207083480403778</v>
+        <v>9.201311023350812</v>
       </c>
       <c r="F14" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G14" t="n">
         <v>1.1</v>
@@ -895,10 +895,10 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>9.207083480403778</v>
+        <v>9.201311023350812</v>
       </c>
       <c r="F15" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G15" t="n">
         <v>1.1</v>
@@ -926,10 +926,10 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>9.207083480403778</v>
+        <v>9.201311023350812</v>
       </c>
       <c r="F16" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -957,10 +957,10 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>12.63751149663229</v>
+        <v>12.62958830439384</v>
       </c>
       <c r="F17" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G17" t="n">
         <v>0.1</v>
@@ -988,10 +988,10 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>12.63751149663229</v>
+        <v>12.62958830439384</v>
       </c>
       <c r="F18" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G18" t="n">
         <v>0.6</v>
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>12.63751149663229</v>
+        <v>12.62958830439384</v>
       </c>
       <c r="F19" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -1050,10 +1050,10 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>12.63751149663229</v>
+        <v>12.62958830439384</v>
       </c>
       <c r="F20" t="n">
-        <v>2.857283911953502</v>
+        <v>2.855492514199263</v>
       </c>
       <c r="G20" t="n">
         <v>1.1</v>
@@ -1081,10 +1081,10 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>14.9244635074513</v>
+        <v>14.91510649175587</v>
       </c>
       <c r="F21" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G21" t="n">
         <v>0.1</v>
@@ -1112,10 +1112,10 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>14.9244635074513</v>
+        <v>14.91510649175587</v>
       </c>
       <c r="F22" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G22" t="n">
         <v>0.6</v>
@@ -1143,10 +1143,10 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>14.9244635074513</v>
+        <v>14.91510649175587</v>
       </c>
       <c r="F23" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
@@ -1174,10 +1174,10 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>14.9244635074513</v>
+        <v>14.91510649175587</v>
       </c>
       <c r="F24" t="n">
-        <v>1.017418571236453</v>
+        <v>1.016780692257745</v>
       </c>
       <c r="G24" t="n">
         <v>1.1</v>
@@ -1205,10 +1205,10 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>13.7809875020418</v>
+        <v>13.77234739807485</v>
       </c>
       <c r="F25" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G25" t="n">
         <v>0.1</v>
@@ -1236,10 +1236,10 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>13.7809875020418</v>
+        <v>13.77234739807485</v>
       </c>
       <c r="F26" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G26" t="n">
         <v>1.1</v>
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>13.7809875020418</v>
+        <v>13.77234739807485</v>
       </c>
       <c r="F27" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G27" t="n">
         <v>1.7</v>
@@ -1298,10 +1298,10 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>13.7809875020418</v>
+        <v>13.77234739807485</v>
       </c>
       <c r="F28" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G28" t="n">
         <v>1.1</v>
@@ -1329,10 +1329,10 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>13.7809875020418</v>
+        <v>13.77234739807485</v>
       </c>
       <c r="F29" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G29" t="n">
         <v>1.1</v>
@@ -1360,10 +1360,10 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>13.7809875020418</v>
+        <v>13.77234739807485</v>
       </c>
       <c r="F30" t="n">
-        <v>1.937351241594977</v>
+        <v>1.936136603228504</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1391,10 +1391,10 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.645330188873331</v>
+        <v>1.644298635518413</v>
       </c>
       <c r="F31" t="n">
-        <v>2.843659757718231</v>
+        <v>2.841876901740046</v>
       </c>
       <c r="G31" t="n">
         <v>0.1</v>
@@ -1422,10 +1422,10 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.645330188873331</v>
+        <v>1.644298635518413</v>
       </c>
       <c r="F32" t="n">
-        <v>2.843659757718231</v>
+        <v>2.841876901740046</v>
       </c>
       <c r="G32" t="n">
         <v>0.6</v>
@@ -1453,10 +1453,10 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1.645330188873331</v>
+        <v>1.644298635518413</v>
       </c>
       <c r="F33" t="n">
-        <v>2.843659757718231</v>
+        <v>2.841876901740046</v>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.645330188873331</v>
+        <v>1.644298635518413</v>
       </c>
       <c r="F34" t="n">
-        <v>2.843659757718231</v>
+        <v>2.841876901740046</v>
       </c>
       <c r="G34" t="n">
         <v>1.1</v>
@@ -1515,10 +1515,10 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3.809826439740048</v>
+        <v>3.807437837578521</v>
       </c>
       <c r="F35" t="n">
-        <v>1.055297951114307</v>
+        <v>1.054636323345442</v>
       </c>
       <c r="G35" t="n">
         <v>0.1</v>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3.809826439740048</v>
+        <v>3.807437837578521</v>
       </c>
       <c r="F36" t="n">
-        <v>1.055297951114307</v>
+        <v>1.054636323345442</v>
       </c>
       <c r="G36" t="n">
         <v>0.6</v>
@@ -1577,10 +1577,10 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3.809826439740048</v>
+        <v>3.807437837578521</v>
       </c>
       <c r="F37" t="n">
-        <v>1.055297951114307</v>
+        <v>1.054636323345442</v>
       </c>
       <c r="G37" t="n">
         <v>1</v>
@@ -1608,10 +1608,10 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>3.809826439740048</v>
+        <v>3.807437837578521</v>
       </c>
       <c r="F38" t="n">
-        <v>1.055297951114307</v>
+        <v>1.054636323345442</v>
       </c>
       <c r="G38" t="n">
         <v>1.1</v>
@@ -1639,10 +1639,10 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2.72757831430669</v>
+        <v>2.725868236548467</v>
       </c>
       <c r="F39" t="n">
-        <v>1.949478854416269</v>
+        <v>1.948256612542744</v>
       </c>
       <c r="G39" t="n">
         <v>0.1</v>
@@ -1670,10 +1670,10 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.72757831430669</v>
+        <v>2.725868236548467</v>
       </c>
       <c r="F40" t="n">
-        <v>1.949478854416269</v>
+        <v>1.948256612542744</v>
       </c>
       <c r="G40" t="n">
         <v>1.1</v>
@@ -1701,10 +1701,10 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2.72757831430669</v>
+        <v>2.725868236548467</v>
       </c>
       <c r="F41" t="n">
-        <v>1.949478854416269</v>
+        <v>1.948256612542744</v>
       </c>
       <c r="G41" t="n">
         <v>1.7</v>
@@ -1732,10 +1732,10 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2.72757831430669</v>
+        <v>2.725868236548467</v>
       </c>
       <c r="F42" t="n">
-        <v>1.949478854416269</v>
+        <v>1.948256612542744</v>
       </c>
       <c r="G42" t="n">
         <v>1.1</v>
@@ -1763,10 +1763,10 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2.72757831430669</v>
+        <v>2.725868236548467</v>
       </c>
       <c r="F43" t="n">
-        <v>1.949478854416269</v>
+        <v>1.948256612542744</v>
       </c>
       <c r="G43" t="n">
         <v>1.1</v>
@@ -1794,10 +1794,10 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2.72757831430669</v>
+        <v>2.725868236548467</v>
       </c>
       <c r="F44" t="n">
-        <v>1.949478854416269</v>
+        <v>1.948256612542744</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -1825,10 +1825,10 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>5.814853340391648</v>
+        <v>5.811207670050094</v>
       </c>
       <c r="F45" t="n">
-        <v>1.860097209756428</v>
+        <v>1.858931006443455</v>
       </c>
       <c r="G45" t="n">
         <v>0.1</v>
@@ -1856,10 +1856,10 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>5.814853340391648</v>
+        <v>5.811207670050094</v>
       </c>
       <c r="F46" t="n">
-        <v>1.860097209756428</v>
+        <v>1.858931006443455</v>
       </c>
       <c r="G46" t="n">
         <v>1.7</v>
@@ -1887,10 +1887,10 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.2865629288199378</v>
+        <v>0.2863832658242556</v>
       </c>
       <c r="F47" t="n">
-        <v>1.893453645449919</v>
+        <v>1.892266529044012</v>
       </c>
       <c r="G47" t="n">
         <v>0.1</v>
@@ -1918,10 +1918,10 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.2865629288199378</v>
+        <v>0.2863832658242556</v>
       </c>
       <c r="F48" t="n">
-        <v>1.893453645449919</v>
+        <v>1.892266529044012</v>
       </c>
       <c r="G48" t="n">
         <v>1.1</v>
@@ -1949,10 +1949,10 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.2865629288199378</v>
+        <v>0.2863832658242556</v>
       </c>
       <c r="F49" t="n">
-        <v>1.893453645449919</v>
+        <v>1.892266529044012</v>
       </c>
       <c r="G49" t="n">
         <v>1.7</v>
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.2865629288199378</v>
+        <v>0.2863832658242556</v>
       </c>
       <c r="F50" t="n">
-        <v>1.893453645449919</v>
+        <v>1.892266529044012</v>
       </c>
       <c r="G50" t="n">
         <v>1.1</v>

</xml_diff>